<commit_message>
Added lookup table functionality to reduce size of chart labels
</commit_message>
<xml_diff>
--- a/outputs/chart_data/All_REF_case_studies_by_discipline.xlsx
+++ b/outputs/chart_data/All_REF_case_studies_by_discipline.xlsx
@@ -25,70 +25,70 @@
     <t>percentage</t>
   </si>
   <si>
-    <t>agricultural_and_veterinary_sciences</t>
-  </si>
-  <si>
-    <t>built_environment_and_design</t>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>earth_sciences</t>
-  </si>
-  <si>
-    <t>environmental_sciences</t>
-  </si>
-  <si>
-    <t>physical_sciences</t>
-  </si>
-  <si>
-    <t>philosophy_and_religious_studies</t>
-  </si>
-  <si>
-    <t>law_and_legal_studies</t>
-  </si>
-  <si>
-    <t>chemical_sciences</t>
-  </si>
-  <si>
-    <t>commerce_management_tourism_and_services</t>
-  </si>
-  <si>
-    <t>education</t>
-  </si>
-  <si>
-    <t>studies_in_creative_arts_and_writing</t>
-  </si>
-  <si>
-    <t>mathematical_sciences</t>
-  </si>
-  <si>
-    <t>psychology_and_cognitive_sciences</t>
-  </si>
-  <si>
-    <t>biological_sciences</t>
-  </si>
-  <si>
-    <t>economics</t>
-  </si>
-  <si>
-    <t>information_and_computing_sciences</t>
-  </si>
-  <si>
-    <t>engineering</t>
-  </si>
-  <si>
-    <t>history_and_archaeology</t>
-  </si>
-  <si>
-    <t>language_communication_and_culture</t>
-  </si>
-  <si>
-    <t>studies_in_human_society</t>
-  </si>
-  <si>
-    <t>medical_and_health_sciences</t>
+    <t>Agri. &amp; Vet sciences</t>
+  </si>
+  <si>
+    <t>Built Env. &amp; Design</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Earth sciences</t>
+  </si>
+  <si>
+    <t>Env. sciences</t>
+  </si>
+  <si>
+    <t>Physical sciences</t>
+  </si>
+  <si>
+    <t>Philo &amp; Relig</t>
+  </si>
+  <si>
+    <t>Law &amp; Legal</t>
+  </si>
+  <si>
+    <t>Chemical sciences</t>
+  </si>
+  <si>
+    <t>Comm. Manage. Tourism</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Creat. Arts &amp; Writing</t>
+  </si>
+  <si>
+    <t>Math sciences</t>
+  </si>
+  <si>
+    <t>Pysch. &amp; Cognit. sciences</t>
+  </si>
+  <si>
+    <t>Biological sciences</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Inf. &amp; Comp. sciences</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Hist. &amp; Archaeology</t>
+  </si>
+  <si>
+    <t>Lang. Comms. &amp; Culture</t>
+  </si>
+  <si>
+    <t>Studies Human Society</t>
+  </si>
+  <si>
+    <t>Med. &amp; Health Sciences</t>
   </si>
 </sst>
 </file>

</xml_diff>